<commit_message>
histogram in dotCSV files done
</commit_message>
<xml_diff>
--- a/PL02/Results.xlsx
+++ b/PL02/Results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
   <si>
     <t>Este documento foi exportado do Numbers. Cada tabela foi convertida numa folha de cálculo Excel. Todos os outros objetos em cada uma das folhas Numbers foram colocados em folhas de cálculo separadas. Tenha presente que os cálculos das fórmulas podem ser diferentes em Excel.</t>
   </si>
@@ -70,13 +70,10 @@
     <t>m (channels)</t>
   </si>
   <si>
-    <t>arrival rate/min</t>
-  </si>
-  <si>
-    <t>arrival rate/hour</t>
-  </si>
-  <si>
-    <t>calls/hour</t>
+    <t>l (arrival rate in min)</t>
+  </si>
+  <si>
+    <t>lambda (calls/hour)</t>
   </si>
   <si>
     <t>dm (min)</t>
@@ -107,10 +104,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="59" formatCode="#,##0.000"/>
-    <numFmt numFmtId="60" formatCode="0.0%"/>
+    <numFmt numFmtId="60" formatCode="#,##0.0"/>
+    <numFmt numFmtId="61" formatCode="0.0%"/>
+    <numFmt numFmtId="62" formatCode="0.000%"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -342,21 +341,18 @@
     <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="59" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="60" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -369,7 +365,10 @@
     <xf numFmtId="9" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="60" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="61" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="62" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -378,7 +377,7 @@
     <xf numFmtId="9" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="60" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="61" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1512,10 +1511,10 @@
     <row r="11">
       <c r="B11" s="4"/>
       <c r="C11" t="s" s="4">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s" s="5">
         <v>24</v>
-      </c>
-      <c r="D11" t="s" s="5">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1534,7 +1533,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:H10"/>
+  <dimension ref="A2:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B4" xSplit="1" ySplit="3" activePane="bottomRight" state="frozen"/>
@@ -1638,31 +1637,27 @@
         <v>18</v>
       </c>
       <c r="B5" s="17">
-        <f>B6/60</f>
+        <f t="shared" si="0" ref="B5:D5">0.009/60</f>
         <v>0.00015</v>
       </c>
       <c r="C5" s="18">
-        <f>C6/60</f>
+        <f t="shared" si="0"/>
         <v>0.00015</v>
       </c>
       <c r="D5" s="18">
-        <f>D6/60</f>
+        <f t="shared" si="0"/>
         <v>0.00015</v>
       </c>
-      <c r="E5" s="18">
-        <f>E6/60</f>
+      <c r="E5" s="19">
         <v>0.001</v>
       </c>
-      <c r="F5" s="18">
-        <f>F6/60</f>
+      <c r="F5" s="19">
         <v>0.001</v>
       </c>
-      <c r="G5" s="18">
-        <f>G6/60</f>
+      <c r="G5" s="19">
         <v>0.001</v>
       </c>
-      <c r="H5" s="18">
-        <f>H6/60</f>
+      <c r="H5" s="20">
         <v>0.2</v>
       </c>
     </row>
@@ -1670,23 +1665,26 @@
       <c r="A6" t="s" s="16">
         <v>19</v>
       </c>
-      <c r="B6" s="19">
-        <v>0.008999999999999999</v>
-      </c>
-      <c r="C6" s="20">
-        <v>0.008999999999999999</v>
-      </c>
-      <c r="D6" s="20">
-        <v>0.008999999999999999</v>
-      </c>
-      <c r="E6" s="21">
-        <v>0.06</v>
-      </c>
-      <c r="F6" s="21">
-        <v>0.06</v>
-      </c>
-      <c r="G6" s="21">
-        <v>0.06</v>
+      <c r="B6" s="21">
+        <f t="shared" si="3" ref="B6:D6">180</f>
+        <v>180</v>
+      </c>
+      <c r="C6" s="22">
+        <f t="shared" si="3"/>
+        <v>180</v>
+      </c>
+      <c r="D6" s="22">
+        <f t="shared" si="3"/>
+        <v>180</v>
+      </c>
+      <c r="E6" s="22">
+        <v>1200</v>
+      </c>
+      <c r="F6" s="22">
+        <v>1200</v>
+      </c>
+      <c r="G6" s="22">
+        <v>1200</v>
       </c>
       <c r="H6" s="22">
         <v>12</v>
@@ -1696,110 +1694,77 @@
       <c r="A7" t="s" s="16">
         <v>20</v>
       </c>
-      <c r="B7" s="23">
-        <f>B6*B10</f>
-        <v>180</v>
+      <c r="B7" s="21">
+        <v>2</v>
       </c>
       <c r="C7" s="22">
-        <f>C6*C10</f>
-        <v>180</v>
+        <v>2</v>
       </c>
       <c r="D7" s="22">
-        <f>D6*D10</f>
-        <v>180</v>
+        <v>2</v>
       </c>
       <c r="E7" s="22">
-        <f>E6*E10</f>
-        <v>1200</v>
+        <v>3</v>
       </c>
       <c r="F7" s="22">
-        <f>F6*F10</f>
-        <v>1200</v>
+        <v>3</v>
       </c>
       <c r="G7" s="22">
-        <f>G6*G10</f>
-        <v>1200</v>
+        <v>3</v>
       </c>
       <c r="H7" s="22">
-        <f>H6*H10</f>
-        <v>240</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" ht="20.05" customHeight="1">
       <c r="A8" t="s" s="16">
         <v>21</v>
       </c>
-      <c r="B8" s="23">
-        <v>2</v>
+      <c r="B8" s="21">
+        <v>0</v>
       </c>
       <c r="C8" s="22">
-        <v>2</v>
+        <v>1000</v>
       </c>
       <c r="D8" s="22">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E8" s="22">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F8" s="22">
-        <v>3</v>
+        <v>1000</v>
       </c>
       <c r="G8" s="22">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H8" s="22">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" ht="20.05" customHeight="1">
       <c r="A9" t="s" s="16">
         <v>22</v>
       </c>
-      <c r="B9" s="23">
-        <v>0</v>
+      <c r="B9" s="21">
+        <v>20000</v>
       </c>
       <c r="C9" s="22">
-        <v>1000</v>
+        <v>20000</v>
       </c>
       <c r="D9" s="22">
-        <v>4</v>
+        <v>20000</v>
       </c>
       <c r="E9" s="22">
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="F9" s="22">
-        <v>1000</v>
+        <v>20000</v>
       </c>
       <c r="G9" s="22">
-        <v>10</v>
+        <v>20000</v>
       </c>
       <c r="H9" s="22">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" t="s" s="16">
-        <v>23</v>
-      </c>
-      <c r="B10" s="23">
-        <v>20000</v>
-      </c>
-      <c r="C10" s="22">
-        <v>20000</v>
-      </c>
-      <c r="D10" s="22">
-        <v>20000</v>
-      </c>
-      <c r="E10" s="22">
-        <v>20000</v>
-      </c>
-      <c r="F10" s="22">
-        <v>20000</v>
-      </c>
-      <c r="G10" s="22">
-        <v>20000</v>
-      </c>
-      <c r="H10" s="22">
         <v>20</v>
       </c>
     </row>
@@ -1831,20 +1796,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="17.8125" style="24" customWidth="1"/>
-    <col min="2" max="2" width="8.61719" style="24" customWidth="1"/>
-    <col min="3" max="3" width="7.25781" style="24" customWidth="1"/>
-    <col min="4" max="4" width="7.35156" style="24" customWidth="1"/>
-    <col min="5" max="5" width="6.17188" style="24" customWidth="1"/>
-    <col min="6" max="6" width="6.40625" style="24" customWidth="1"/>
-    <col min="7" max="7" width="6.40625" style="24" customWidth="1"/>
-    <col min="8" max="8" width="11" style="24" customWidth="1"/>
-    <col min="9" max="256" width="16.3516" style="24" customWidth="1"/>
+    <col min="1" max="1" width="17.8125" style="23" customWidth="1"/>
+    <col min="2" max="2" width="8.61719" style="23" customWidth="1"/>
+    <col min="3" max="3" width="7.25781" style="23" customWidth="1"/>
+    <col min="4" max="4" width="7.35156" style="23" customWidth="1"/>
+    <col min="5" max="5" width="6.17188" style="23" customWidth="1"/>
+    <col min="6" max="6" width="6.40625" style="23" customWidth="1"/>
+    <col min="7" max="7" width="6.40625" style="23" customWidth="1"/>
+    <col min="8" max="8" width="11" style="23" customWidth="1"/>
+    <col min="9" max="256" width="16.3516" style="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
       <c r="A1" t="s" s="7">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -1897,34 +1862,34 @@
       </c>
     </row>
     <row r="4" ht="20.25" customHeight="1">
-      <c r="A4" t="s" s="25">
-        <v>26</v>
-      </c>
-      <c r="B4" s="26">
+      <c r="A4" t="s" s="24">
+        <v>25</v>
+      </c>
+      <c r="B4" s="25">
         <v>0.12</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="26">
         <v>0</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D4" s="27">
         <v>0.031</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="27">
         <v>0.059</v>
       </c>
-      <c r="F4" s="27">
+      <c r="F4" s="26">
         <v>0</v>
       </c>
-      <c r="G4" s="27">
+      <c r="G4" s="26">
         <v>0.02</v>
       </c>
       <c r="H4" s="28">
-        <v>0.054</v>
+        <v>0.00514</v>
       </c>
     </row>
     <row r="5" ht="20.05" customHeight="1">
       <c r="A5" t="s" s="29">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="30">
         <v>0</v>
@@ -1950,7 +1915,7 @@
     </row>
     <row r="6" ht="20.05" customHeight="1">
       <c r="A6" t="s" s="29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="17">
         <v>0</v>

</xml_diff>